<commit_message>
Updated file with latest changes
</commit_message>
<xml_diff>
--- a/Booking_Merged.xlsx
+++ b/Booking_Merged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\tuda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0306D6FE-2639-4D30-8B44-9598A7547BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4142BB15-F2E0-407A-89EE-E1E9CD65B70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C520B2EF-914A-46B0-A9F8-3B0CF775724D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$82</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$81</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -48,46 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="255">
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
-  <si>
-    <t>hotel_name</t>
-  </si>
-  <si>
-    <t>locality</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>score</t>
-  </si>
-  <si>
-    <t>review</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="249">
   <si>
     <t>Gold Park 3BR Apartment</t>
   </si>
@@ -813,6 +774,27 @@
   </si>
   <si>
     <t>Hideaway homesa</t>
+  </si>
+  <si>
+    <t>No of Reviews</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Locality</t>
+  </si>
+  <si>
+    <t>Hotel_name</t>
   </si>
 </sst>
 </file>
@@ -912,8 +894,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62167563-DC3E-4A75-9866-2E3125A1968A}" name="Booking_com" displayName="Booking_com" ref="A1:G82" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G82" xr:uid="{62167563-DC3E-4A75-9866-2E3125A1968A}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62167563-DC3E-4A75-9866-2E3125A1968A}" name="Booking_com" displayName="Booking_com" ref="A1:G81" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G81" xr:uid="{62167563-DC3E-4A75-9866-2E3125A1968A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -923,13 +905,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="8" xr3:uid="{EFBD94A6-AFEA-4221-A20C-3778D46CE75F}" uniqueName="8" name="Column1" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DBE72513-99D0-4B58-915D-8F7BF97151DE}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{0E92F78B-DA54-48C9-B6EB-90A23EF39F26}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{D50F57C1-4D70-44EC-ACA8-F6D09F8EC73A}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{B2421D85-2F20-42C0-A98D-D26950BEBA0A}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{137D2C92-6C3B-47C1-ABF0-278B8856503D}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{86ED90A9-F32A-4AAE-95DA-1DAEAD0B44F2}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{EFBD94A6-AFEA-4221-A20C-3778D46CE75F}" uniqueName="8" name="Hotel_name" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DBE72513-99D0-4B58-915D-8F7BF97151DE}" uniqueName="2" name="Locality" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{0E92F78B-DA54-48C9-B6EB-90A23EF39F26}" uniqueName="3" name="Price" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{D50F57C1-4D70-44EC-ACA8-F6D09F8EC73A}" uniqueName="4" name="Rating" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{B2421D85-2F20-42C0-A98D-D26950BEBA0A}" uniqueName="5" name="Score" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{137D2C92-6C3B-47C1-ABF0-278B8856503D}" uniqueName="6" name="No of Reviews" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{86ED90A9-F32A-4AAE-95DA-1DAEAD0B44F2}" uniqueName="7" name="Reviews" queryTableFieldId="7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1232,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422F8FE1-2074-4320-9FE3-023EC79E52AB}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,50 +1228,50 @@
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>247</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>246</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>245</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>244</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>242</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G2" t="e">
         <f>VLOOKUP(A2,#REF!, 2, FALSE)</f>
@@ -1298,22 +1280,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G3" t="e">
         <f>VLOOKUP(A3,#REF!, 2, FALSE)</f>
@@ -1322,22 +1304,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G4" t="e">
         <f>VLOOKUP(A4,#REF!, 2, FALSE)</f>
@@ -1346,22 +1328,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G5" t="e">
         <f>VLOOKUP(A5,#REF!, 2, FALSE)</f>
@@ -1370,22 +1352,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
       </c>
       <c r="G6" t="e">
         <f>VLOOKUP(A6,#REF!, 2, FALSE)</f>
@@ -1394,22 +1376,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G7" t="e">
         <f>VLOOKUP(A7,#REF!, 2, FALSE)</f>
@@ -1418,22 +1400,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G8" t="e">
         <f>VLOOKUP(A8,#REF!, 2, FALSE)</f>
@@ -1442,22 +1424,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="G9" t="e">
         <f>VLOOKUP(A9,#REF!, 2, FALSE)</f>
@@ -1466,22 +1448,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G10" t="e">
         <f>VLOOKUP(A10,#REF!, 2, FALSE)</f>
@@ -1490,22 +1472,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G11" t="e">
         <f>VLOOKUP(A11,#REF!, 2, FALSE)</f>
@@ -1514,22 +1496,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G12" t="e">
         <f>VLOOKUP(A12,#REF!, 2, FALSE)</f>
@@ -1538,22 +1520,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
-        <v>53</v>
-      </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G13" t="e">
         <f>VLOOKUP(A13,#REF!, 2, FALSE)</f>
@@ -1562,22 +1544,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G14" t="e">
         <f>VLOOKUP(A14,#REF!, 2, FALSE)</f>
@@ -1586,22 +1568,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G15" t="e">
         <f>VLOOKUP(A15,#REF!, 2, FALSE)</f>
@@ -1610,22 +1592,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="G16" t="e">
         <f>VLOOKUP(A16,#REF!, 2, FALSE)</f>
@@ -1634,22 +1616,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G17" t="e">
         <f>VLOOKUP(A17,#REF!, 2, FALSE)</f>
@@ -1658,22 +1640,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G18" t="e">
         <f>VLOOKUP(A18,#REF!, 2, FALSE)</f>
@@ -1682,22 +1664,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G19" t="e">
         <f>VLOOKUP(A19,#REF!, 2, FALSE)</f>
@@ -1706,22 +1688,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G20" t="e">
         <f>VLOOKUP(A20,#REF!, 2, FALSE)</f>
@@ -1730,22 +1712,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G21" t="e">
         <f>VLOOKUP(A21,#REF!, 2, FALSE)</f>
@@ -1754,22 +1736,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G22" t="e">
         <f>VLOOKUP(A22,#REF!, 2, FALSE)</f>
@@ -1778,22 +1760,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="G23" t="e">
         <f>VLOOKUP(A23,#REF!, 2, FALSE)</f>
@@ -1802,22 +1784,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="G24" t="e">
         <f>VLOOKUP(A24,#REF!, 2, FALSE)</f>
@@ -1826,22 +1808,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="F25" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="G25" t="e">
         <f>VLOOKUP(A25,#REF!, 2, FALSE)</f>
@@ -1850,22 +1832,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="G26" t="e">
         <f>VLOOKUP(A26,#REF!, 2, FALSE)</f>
@@ -1874,22 +1856,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="F27" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="G27" t="e">
         <f>VLOOKUP(A27,#REF!, 2, FALSE)</f>
@@ -1898,22 +1880,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G28" t="e">
         <f>VLOOKUP(A28,#REF!, 2, FALSE)</f>
@@ -1922,22 +1904,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G29" t="e">
         <f>VLOOKUP(A29,#REF!, 2, FALSE)</f>
@@ -1946,22 +1928,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G30" t="e">
         <f>VLOOKUP(A30,#REF!, 2, FALSE)</f>
@@ -1970,22 +1952,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G31" t="e">
         <f>VLOOKUP(A31,#REF!, 2, FALSE)</f>
@@ -1994,22 +1976,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="F32" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="G32" t="e">
         <f>VLOOKUP(A32,#REF!, 2, FALSE)</f>
@@ -2018,22 +2000,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F33" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G33" t="e">
         <f>VLOOKUP(A33,#REF!, 2, FALSE)</f>
@@ -2042,22 +2024,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F34" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="G34" t="e">
         <f>VLOOKUP(A34,#REF!, 2, FALSE)</f>
@@ -2066,22 +2048,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="E35" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F35" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="G35" t="e">
         <f>VLOOKUP(A35,#REF!, 2, FALSE)</f>
@@ -2090,22 +2072,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E36" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F36" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="G36" t="e">
         <f>VLOOKUP(A36,#REF!, 2, FALSE)</f>
@@ -2114,22 +2096,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="F37" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G37" t="e">
         <f>VLOOKUP(A37,#REF!, 2, FALSE)</f>
@@ -2138,22 +2120,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G38" t="e">
         <f>VLOOKUP(A38,#REF!, 2, FALSE)</f>
@@ -2162,22 +2144,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="F39" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G39" t="e">
         <f>VLOOKUP(A39,#REF!, 2, FALSE)</f>
@@ -2186,22 +2168,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E40" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F40" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G40" t="e">
         <f>VLOOKUP(A40,#REF!, 2, FALSE)</f>
@@ -2210,22 +2192,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F41" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G41" t="e">
         <f>VLOOKUP(A41,#REF!, 2, FALSE)</f>
@@ -2234,22 +2216,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="F42" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="G42" t="e">
         <f>VLOOKUP(A42,#REF!, 2, FALSE)</f>
@@ -2258,22 +2240,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E43" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F43" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="G43" t="e">
         <f>VLOOKUP(A43,#REF!, 2, FALSE)</f>
@@ -2282,22 +2264,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E44" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F44" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="G44" t="e">
         <f>VLOOKUP(A44,#REF!, 2, FALSE)</f>
@@ -2306,22 +2288,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E45" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F45" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="G45" t="e">
         <f>VLOOKUP(A45,#REF!, 2, FALSE)</f>
@@ -2330,22 +2312,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E46" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F46" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="G46" t="e">
         <f>VLOOKUP(A46,#REF!, 2, FALSE)</f>
@@ -2354,22 +2336,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="F47" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G47" t="e">
         <f>VLOOKUP(A47,#REF!, 2, FALSE)</f>
@@ -2378,22 +2360,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D48" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F48" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G48" t="e">
         <f>VLOOKUP(A48,#REF!, 2, FALSE)</f>
@@ -2402,22 +2384,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D49" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E49" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F49" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="G49" t="e">
         <f>VLOOKUP(A49,#REF!, 2, FALSE)</f>
@@ -2426,22 +2408,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D50" t="s">
-        <v>169</v>
+        <v>26</v>
       </c>
       <c r="E50" t="s">
-        <v>170</v>
+        <v>26</v>
       </c>
       <c r="F50" t="s">
-        <v>171</v>
+        <v>27</v>
       </c>
       <c r="G50" t="e">
         <f>VLOOKUP(A50,#REF!, 2, FALSE)</f>
@@ -2450,22 +2432,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D51" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="G51" t="e">
         <f>VLOOKUP(A51,#REF!, 2, FALSE)</f>
@@ -2474,22 +2456,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>175</v>
+        <v>66</v>
       </c>
       <c r="D52" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="F52" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="G52" t="e">
         <f>VLOOKUP(A52,#REF!, 2, FALSE)</f>
@@ -2498,22 +2480,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>79</v>
+        <v>167</v>
       </c>
       <c r="D53" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="F53" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="G53" t="e">
         <f>VLOOKUP(A53,#REF!, 2, FALSE)</f>
@@ -2522,22 +2504,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
       <c r="D54" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="E54" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="F54" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G54" t="e">
         <f>VLOOKUP(A54,#REF!, 2, FALSE)</f>
@@ -2546,22 +2528,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C55" t="s">
-        <v>68</v>
+        <v>173</v>
       </c>
       <c r="D55" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E55" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F55" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G55" t="e">
         <f>VLOOKUP(A55,#REF!, 2, FALSE)</f>
@@ -2570,22 +2552,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D56" t="s">
-        <v>169</v>
+        <v>26</v>
       </c>
       <c r="E56" t="s">
-        <v>187</v>
+        <v>26</v>
       </c>
       <c r="F56" t="s">
-        <v>188</v>
+        <v>27</v>
       </c>
       <c r="G56" t="e">
         <f>VLOOKUP(A56,#REF!, 2, FALSE)</f>
@@ -2594,22 +2576,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D57" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E57" t="s">
-        <v>39</v>
+        <v>180</v>
       </c>
       <c r="F57" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="G57" t="e">
         <f>VLOOKUP(A57,#REF!, 2, FALSE)</f>
@@ -2618,22 +2600,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C58" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D58" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E58" t="s">
-        <v>193</v>
+        <v>110</v>
       </c>
       <c r="F58" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="G58" t="e">
         <f>VLOOKUP(A58,#REF!, 2, FALSE)</f>
@@ -2642,22 +2624,22 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C59" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D59" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="E59" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="F59" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
       <c r="G59" t="e">
         <f>VLOOKUP(A59,#REF!, 2, FALSE)</f>
@@ -2666,22 +2648,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="C60" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D60" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E60" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F60" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="G60" t="e">
         <f>VLOOKUP(A60,#REF!, 2, FALSE)</f>
@@ -2690,22 +2672,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D61" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="E61" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F61" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="G61" t="e">
         <f>VLOOKUP(A61,#REF!, 2, FALSE)</f>
@@ -2714,22 +2696,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D62" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="E62" t="s">
-        <v>207</v>
+        <v>48</v>
       </c>
       <c r="F62" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="G62" t="e">
         <f>VLOOKUP(A62,#REF!, 2, FALSE)</f>
@@ -2738,22 +2720,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C63" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D63" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E63" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="G63" t="e">
         <f>VLOOKUP(A63,#REF!, 2, FALSE)</f>
@@ -2762,22 +2744,22 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D64" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E64" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="F64" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="G64" t="e">
         <f>VLOOKUP(A64,#REF!, 2, FALSE)</f>
@@ -2786,22 +2768,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E65" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="F65" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G65" t="e">
         <f>VLOOKUP(A65,#REF!, 2, FALSE)</f>
@@ -2810,22 +2792,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D66" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="E66" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="F66" t="s">
-        <v>219</v>
+        <v>27</v>
       </c>
       <c r="G66" t="e">
         <f>VLOOKUP(A66,#REF!, 2, FALSE)</f>
@@ -2834,22 +2816,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B67" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="D67" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="E67" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="F67" t="s">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="G67" t="e">
         <f>VLOOKUP(A67,#REF!, 2, FALSE)</f>
@@ -2858,22 +2840,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D68" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="E68" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="F68" t="s">
-        <v>224</v>
+        <v>27</v>
       </c>
       <c r="G68" t="e">
         <f>VLOOKUP(A68,#REF!, 2, FALSE)</f>
@@ -2882,22 +2864,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D69" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="E69" t="s">
-        <v>39</v>
+        <v>157</v>
       </c>
       <c r="F69" t="s">
-        <v>40</v>
+        <v>216</v>
       </c>
       <c r="G69" t="e">
         <f>VLOOKUP(A69,#REF!, 2, FALSE)</f>
@@ -2906,22 +2888,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B70" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D70" t="s">
-        <v>169</v>
+        <v>9</v>
       </c>
       <c r="E70" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="F70" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="G70" t="e">
         <f>VLOOKUP(A70,#REF!, 2, FALSE)</f>
@@ -2930,22 +2912,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B71" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C71" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D71" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E71" t="s">
-        <v>140</v>
+        <v>26</v>
       </c>
       <c r="F71" t="s">
-        <v>232</v>
+        <v>27</v>
       </c>
       <c r="G71" t="e">
         <f>VLOOKUP(A71,#REF!, 2, FALSE)</f>
@@ -2954,22 +2936,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D72" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E72" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F72" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G72" t="e">
         <f>VLOOKUP(A72,#REF!, 2, FALSE)</f>
@@ -2978,22 +2960,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B73" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="D73" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E73" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F73" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G73" t="e">
         <f>VLOOKUP(A73,#REF!, 2, FALSE)</f>
@@ -3002,22 +2984,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B74" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C74" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D74" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E74" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F74" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G74" t="e">
         <f>VLOOKUP(A74,#REF!, 2, FALSE)</f>
@@ -3026,22 +3008,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B75" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D75" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E75" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F75" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G75" t="e">
         <f>VLOOKUP(A75,#REF!, 2, FALSE)</f>
@@ -3050,22 +3032,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C76" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="D76" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E76" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F76" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G76" t="e">
         <f>VLOOKUP(A76,#REF!, 2, FALSE)</f>
@@ -3074,22 +3056,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B77" t="s">
-        <v>42</v>
+        <v>233</v>
       </c>
       <c r="C77" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D77" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E77" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F77" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G77" t="e">
         <f>VLOOKUP(A77,#REF!, 2, FALSE)</f>
@@ -3098,22 +3080,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>29</v>
       </c>
       <c r="C78" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="D78" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E78" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F78" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G78" t="e">
         <f>VLOOKUP(A78,#REF!, 2, FALSE)</f>
@@ -3122,22 +3104,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B79" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D79" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E79" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F79" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G79" t="e">
         <f>VLOOKUP(A79,#REF!, 2, FALSE)</f>
@@ -3146,22 +3128,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="D80" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E80" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F80" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G80" t="e">
         <f>VLOOKUP(A80,#REF!, 2, FALSE)</f>
@@ -3170,49 +3152,25 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C81" t="s">
-        <v>253</v>
+        <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E81" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F81" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G81" t="e">
         <f>VLOOKUP(A81,#REF!, 2, FALSE)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>254</v>
-      </c>
-      <c r="B82" t="s">
-        <v>42</v>
-      </c>
-      <c r="C82" t="s">
-        <v>31</v>
-      </c>
-      <c r="D82" t="s">
-        <v>39</v>
-      </c>
-      <c r="E82" t="s">
-        <v>39</v>
-      </c>
-      <c r="F82" t="s">
-        <v>40</v>
-      </c>
-      <c r="G82" t="e">
-        <f>VLOOKUP(A82,#REF!, 2, FALSE)</f>
         <v>#REF!</v>
       </c>
     </row>

</xml_diff>